<commit_message>
add sx1268 and modify sensor driver
</commit_message>
<xml_diff>
--- a/sensor/协议.xlsx
+++ b/sensor/协议.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9924"/>
+    <workbookView windowWidth="21000" windowHeight="8555"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>数据结构</t>
   </si>
@@ -109,11 +109,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,30 +130,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,15 +181,71 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,30 +261,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -229,61 +268,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -298,31 +283,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,7 +391,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,13 +427,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,115 +457,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,11 +492,70 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,15 +575,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -554,66 +589,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -622,137 +607,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,14 +746,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1093,8 +1074,8 @@
   <sheetPr/>
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -1156,7 +1137,7 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="3">
@@ -1195,30 +1176,30 @@
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="5"/>
+      <c r="A4" s="4"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="5"/>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="5"/>
+      <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="5"/>
+      <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="5"/>
+      <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
@@ -1226,7 +1207,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
@@ -1234,80 +1215,80 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>